<commit_message>
Getting all main branch up to date before looking at main - refactor
</commit_message>
<xml_diff>
--- a/Test Strategy.xlsx
+++ b/Test Strategy.xlsx
@@ -8,14 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/79738e9b9c1f34f3/MSc/41670 Software Engineering/Group_Project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="142" documentId="8_{B813F0D1-8B60-4A61-9B7A-E5FE2B6792D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{03CFCA12-0182-4B20-BF73-C5ECB4EBBBC2}"/>
+  <xr:revisionPtr revIDLastSave="299" documentId="8_{B813F0D1-8B60-4A61-9B7A-E5FE2B6792D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{05C119DD-1752-4057-8FC0-6A6386050012}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{CC64A86E-5228-4C9F-A273-8C9B43EE2FC5}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="5" xr2:uid="{CC64A86E-5228-4C9F-A273-8C9B43EE2FC5}"/>
   </bookViews>
   <sheets>
     <sheet name="Point" sheetId="1" r:id="rId1"/>
     <sheet name="OffBoard" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet1" sheetId="3" r:id="rId3"/>
+    <sheet name="Board" sheetId="4" r:id="rId3"/>
+    <sheet name="Player" sheetId="5" r:id="rId4"/>
+    <sheet name="Board Layout" sheetId="3" r:id="rId5"/>
+    <sheet name="Sheet6" sheetId="8" r:id="rId6"/>
+    <sheet name="Weird scenario" sheetId="6" r:id="rId7"/>
+    <sheet name="canClear" sheetId="7" r:id="rId8"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="314" uniqueCount="136">
   <si>
     <t>Class</t>
   </si>
@@ -355,6 +360,102 @@
   </si>
   <si>
     <t>6,13</t>
+  </si>
+  <si>
+    <t>Board</t>
+  </si>
+  <si>
+    <t>Normal point</t>
+  </si>
+  <si>
+    <t>Normal point, has pieces</t>
+  </si>
+  <si>
+    <t>Returns the top piece, removes the top piece from that stack</t>
+  </si>
+  <si>
+    <t>Bar, has pieces of the relevant colour</t>
+  </si>
+  <si>
+    <t>Off</t>
+  </si>
+  <si>
+    <t>Returns null - can't remove pieces from off board</t>
+  </si>
+  <si>
+    <t>Normal point, no pieces</t>
+  </si>
+  <si>
+    <t>Bar, has no pieces of relevant colour</t>
+  </si>
+  <si>
+    <t>setColour</t>
+  </si>
+  <si>
+    <t>Off or Bar point</t>
+  </si>
+  <si>
+    <t>Colour set by parameter</t>
+  </si>
+  <si>
+    <t>IndexOutofBounds exception</t>
+  </si>
+  <si>
+    <t>placePieces</t>
+  </si>
+  <si>
+    <t>Board set up with pieces on expected locations</t>
+  </si>
+  <si>
+    <t>Player</t>
+  </si>
+  <si>
+    <t>getPipScore</t>
+  </si>
+  <si>
+    <t>Sum of pip values for every piece</t>
+  </si>
+  <si>
+    <t>Start position</t>
+  </si>
+  <si>
+    <t>Some moves</t>
+  </si>
+  <si>
+    <t>Black Checkers</t>
+  </si>
+  <si>
+    <t>White Checkers</t>
+  </si>
+  <si>
+    <t>Black rolls 3,5</t>
+  </si>
+  <si>
+    <t>From</t>
+  </si>
+  <si>
+    <t>To</t>
+  </si>
+  <si>
+    <t>Select move 1</t>
+  </si>
+  <si>
+    <t>Legal moves with 3</t>
+  </si>
+  <si>
+    <t>Select move 2</t>
+  </si>
+  <si>
+    <t>Select move 3</t>
+  </si>
+  <si>
+    <t>No valid moves!</t>
+  </si>
+  <si>
+    <t>Select move 4</t>
+  </si>
+  <si>
+    <t>It doesn't always take the different die on the second move</t>
   </si>
 </sst>
 </file>
@@ -425,6 +526,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1025,8 +1130,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{945A7F1C-5A15-42E9-9C86-01CF3F6289C2}">
   <dimension ref="A1:E47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="D31" sqref="C28:D31"/>
+    <sheetView topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="C39" sqref="C39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1498,11 +1603,197 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{95D0E82E-F203-46D6-BDC0-063DBCFC77DB}">
+  <dimension ref="A1:D9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="34.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="56" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>104</v>
+      </c>
+      <c r="B2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C3" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C4" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C5" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C6" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>113</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C8" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>117</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>118</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2D5F749B-A813-4021-92C6-12D9E33BA9E8}">
+  <dimension ref="A1:D24"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="34.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="56" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>119</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C3" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="5" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="6" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="7" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="8" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="9" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="10" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="11" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="12" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="13" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="14" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="15" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="16" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="17" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="18" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="19" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="20" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="21" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="22" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="23" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="24" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B515B96F-2134-4073-ABAF-41B06F4B1686}">
   <dimension ref="A1:S16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="S5" sqref="S5"/>
+      <selection sqref="A1:XFD16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1559,7 +1850,7 @@
         <v>23</v>
       </c>
       <c r="Q3">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="S3">
         <v>25</v>
@@ -1997,6 +2288,1900 @@
       </c>
       <c r="S16" t="s">
         <v>97</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F36F80C-CC17-460E-AC0E-2F5195118961}">
+  <dimension ref="A1:S24"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J9" sqref="J9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="15" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>94</v>
+      </c>
+      <c r="J1" t="s">
+        <v>98</v>
+      </c>
+      <c r="S1" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>88</v>
+      </c>
+      <c r="C3">
+        <v>13</v>
+      </c>
+      <c r="D3">
+        <v>14</v>
+      </c>
+      <c r="E3">
+        <v>15</v>
+      </c>
+      <c r="F3">
+        <v>16</v>
+      </c>
+      <c r="G3">
+        <v>17</v>
+      </c>
+      <c r="H3">
+        <v>18</v>
+      </c>
+      <c r="J3">
+        <v>0</v>
+      </c>
+      <c r="L3">
+        <v>19</v>
+      </c>
+      <c r="M3">
+        <v>20</v>
+      </c>
+      <c r="N3">
+        <v>21</v>
+      </c>
+      <c r="O3">
+        <v>22</v>
+      </c>
+      <c r="P3">
+        <v>23</v>
+      </c>
+      <c r="Q3">
+        <v>24</v>
+      </c>
+      <c r="S3">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>89</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+      <c r="E4">
+        <v>1</v>
+      </c>
+      <c r="F4">
+        <v>1</v>
+      </c>
+      <c r="G4">
+        <v>1</v>
+      </c>
+      <c r="H4">
+        <v>1</v>
+      </c>
+      <c r="J4">
+        <v>1</v>
+      </c>
+      <c r="L4">
+        <v>1</v>
+      </c>
+      <c r="M4">
+        <v>1</v>
+      </c>
+      <c r="N4">
+        <v>1</v>
+      </c>
+      <c r="O4">
+        <v>1</v>
+      </c>
+      <c r="P4">
+        <v>1</v>
+      </c>
+      <c r="Q4">
+        <v>1</v>
+      </c>
+      <c r="S4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>90</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+      <c r="E5">
+        <v>2</v>
+      </c>
+      <c r="F5">
+        <v>3</v>
+      </c>
+      <c r="G5">
+        <v>4</v>
+      </c>
+      <c r="H5">
+        <v>5</v>
+      </c>
+      <c r="J5">
+        <v>6</v>
+      </c>
+      <c r="L5">
+        <v>7</v>
+      </c>
+      <c r="M5">
+        <v>8</v>
+      </c>
+      <c r="N5">
+        <v>9</v>
+      </c>
+      <c r="O5">
+        <v>10</v>
+      </c>
+      <c r="P5">
+        <v>11</v>
+      </c>
+      <c r="Q5">
+        <v>12</v>
+      </c>
+      <c r="S5">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>91</v>
+      </c>
+      <c r="C6">
+        <v>12</v>
+      </c>
+      <c r="D6">
+        <v>11</v>
+      </c>
+      <c r="E6">
+        <v>10</v>
+      </c>
+      <c r="F6">
+        <v>9</v>
+      </c>
+      <c r="G6">
+        <v>8</v>
+      </c>
+      <c r="H6">
+        <v>7</v>
+      </c>
+      <c r="J6">
+        <v>25</v>
+      </c>
+      <c r="L6">
+        <v>6</v>
+      </c>
+      <c r="M6">
+        <v>5</v>
+      </c>
+      <c r="N6">
+        <v>4</v>
+      </c>
+      <c r="O6">
+        <v>3</v>
+      </c>
+      <c r="P6">
+        <v>2</v>
+      </c>
+      <c r="Q6">
+        <v>1</v>
+      </c>
+      <c r="S6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>92</v>
+      </c>
+      <c r="C7">
+        <v>13</v>
+      </c>
+      <c r="D7">
+        <v>14</v>
+      </c>
+      <c r="E7">
+        <v>15</v>
+      </c>
+      <c r="F7">
+        <v>16</v>
+      </c>
+      <c r="G7">
+        <v>17</v>
+      </c>
+      <c r="H7">
+        <v>18</v>
+      </c>
+      <c r="J7" t="s">
+        <v>95</v>
+      </c>
+      <c r="L7">
+        <v>19</v>
+      </c>
+      <c r="M7">
+        <v>20</v>
+      </c>
+      <c r="N7">
+        <v>21</v>
+      </c>
+      <c r="O7">
+        <v>22</v>
+      </c>
+      <c r="P7">
+        <v>23</v>
+      </c>
+      <c r="Q7">
+        <v>25</v>
+      </c>
+      <c r="S7" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>124</v>
+      </c>
+      <c r="D8">
+        <v>2</v>
+      </c>
+      <c r="G8">
+        <v>3</v>
+      </c>
+      <c r="J8">
+        <v>1</v>
+      </c>
+      <c r="L8">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>125</v>
+      </c>
+      <c r="C9">
+        <v>2</v>
+      </c>
+      <c r="H9">
+        <v>1</v>
+      </c>
+      <c r="Q9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>125</v>
+      </c>
+      <c r="D10">
+        <v>1</v>
+      </c>
+      <c r="F10">
+        <v>1</v>
+      </c>
+      <c r="G10">
+        <v>4</v>
+      </c>
+      <c r="L10">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>124</v>
+      </c>
+      <c r="C11">
+        <v>2</v>
+      </c>
+      <c r="Q11">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>88</v>
+      </c>
+      <c r="C12">
+        <v>12</v>
+      </c>
+      <c r="D12">
+        <v>11</v>
+      </c>
+      <c r="E12">
+        <v>10</v>
+      </c>
+      <c r="F12">
+        <v>9</v>
+      </c>
+      <c r="G12">
+        <v>8</v>
+      </c>
+      <c r="H12">
+        <v>7</v>
+      </c>
+      <c r="J12">
+        <v>25</v>
+      </c>
+      <c r="L12">
+        <v>6</v>
+      </c>
+      <c r="M12">
+        <v>5</v>
+      </c>
+      <c r="N12">
+        <v>4</v>
+      </c>
+      <c r="O12">
+        <v>3</v>
+      </c>
+      <c r="P12">
+        <v>2</v>
+      </c>
+      <c r="Q12">
+        <v>1</v>
+      </c>
+      <c r="S12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>89</v>
+      </c>
+      <c r="C13">
+        <v>13</v>
+      </c>
+      <c r="D13">
+        <v>13</v>
+      </c>
+      <c r="E13">
+        <v>13</v>
+      </c>
+      <c r="F13">
+        <v>13</v>
+      </c>
+      <c r="G13">
+        <v>13</v>
+      </c>
+      <c r="H13">
+        <v>13</v>
+      </c>
+      <c r="J13">
+        <v>13</v>
+      </c>
+      <c r="L13">
+        <v>13</v>
+      </c>
+      <c r="M13">
+        <v>13</v>
+      </c>
+      <c r="N13">
+        <v>13</v>
+      </c>
+      <c r="O13">
+        <v>13</v>
+      </c>
+      <c r="P13">
+        <v>13</v>
+      </c>
+      <c r="Q13">
+        <v>13</v>
+      </c>
+      <c r="S13">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>90</v>
+      </c>
+      <c r="C14">
+        <v>0</v>
+      </c>
+      <c r="D14">
+        <v>1</v>
+      </c>
+      <c r="E14">
+        <v>2</v>
+      </c>
+      <c r="F14">
+        <v>3</v>
+      </c>
+      <c r="G14">
+        <v>4</v>
+      </c>
+      <c r="H14">
+        <v>5</v>
+      </c>
+      <c r="J14">
+        <v>6</v>
+      </c>
+      <c r="L14">
+        <v>7</v>
+      </c>
+      <c r="M14">
+        <v>8</v>
+      </c>
+      <c r="N14">
+        <v>9</v>
+      </c>
+      <c r="O14">
+        <v>10</v>
+      </c>
+      <c r="P14">
+        <v>11</v>
+      </c>
+      <c r="Q14">
+        <v>12</v>
+      </c>
+      <c r="S14">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>91</v>
+      </c>
+      <c r="C15">
+        <v>13</v>
+      </c>
+      <c r="D15">
+        <v>14</v>
+      </c>
+      <c r="E15">
+        <v>15</v>
+      </c>
+      <c r="F15">
+        <v>16</v>
+      </c>
+      <c r="G15">
+        <v>17</v>
+      </c>
+      <c r="H15">
+        <v>18</v>
+      </c>
+      <c r="J15" t="s">
+        <v>95</v>
+      </c>
+      <c r="L15">
+        <v>19</v>
+      </c>
+      <c r="M15">
+        <v>20</v>
+      </c>
+      <c r="N15">
+        <v>21</v>
+      </c>
+      <c r="O15">
+        <v>22</v>
+      </c>
+      <c r="P15">
+        <v>23</v>
+      </c>
+      <c r="Q15">
+        <v>24</v>
+      </c>
+      <c r="S15" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>92</v>
+      </c>
+      <c r="C16">
+        <v>12</v>
+      </c>
+      <c r="D16">
+        <v>11</v>
+      </c>
+      <c r="E16">
+        <v>10</v>
+      </c>
+      <c r="F16">
+        <v>9</v>
+      </c>
+      <c r="G16">
+        <v>8</v>
+      </c>
+      <c r="H16">
+        <v>7</v>
+      </c>
+      <c r="J16">
+        <v>25</v>
+      </c>
+      <c r="L16">
+        <v>6</v>
+      </c>
+      <c r="M16">
+        <v>5</v>
+      </c>
+      <c r="N16">
+        <v>4</v>
+      </c>
+      <c r="O16">
+        <v>3</v>
+      </c>
+      <c r="P16">
+        <v>2</v>
+      </c>
+      <c r="Q16">
+        <v>1</v>
+      </c>
+      <c r="S16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>93</v>
+      </c>
+      <c r="J18" t="s">
+        <v>96</v>
+      </c>
+      <c r="S18" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="24" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="C24" t="s">
+        <v>135</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9296555F-9967-4940-8237-019CDB589D0F}">
+  <dimension ref="A1:S35"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>94</v>
+      </c>
+      <c r="J1" t="s">
+        <v>98</v>
+      </c>
+      <c r="S1" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>88</v>
+      </c>
+      <c r="C3">
+        <v>13</v>
+      </c>
+      <c r="D3">
+        <v>14</v>
+      </c>
+      <c r="E3">
+        <v>15</v>
+      </c>
+      <c r="F3">
+        <v>16</v>
+      </c>
+      <c r="G3">
+        <v>17</v>
+      </c>
+      <c r="H3">
+        <v>18</v>
+      </c>
+      <c r="J3">
+        <v>0</v>
+      </c>
+      <c r="L3">
+        <v>19</v>
+      </c>
+      <c r="M3">
+        <v>20</v>
+      </c>
+      <c r="N3">
+        <v>21</v>
+      </c>
+      <c r="O3">
+        <v>22</v>
+      </c>
+      <c r="P3">
+        <v>23</v>
+      </c>
+      <c r="Q3">
+        <v>24</v>
+      </c>
+      <c r="S3">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>89</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+      <c r="E4">
+        <v>1</v>
+      </c>
+      <c r="F4">
+        <v>1</v>
+      </c>
+      <c r="G4">
+        <v>1</v>
+      </c>
+      <c r="H4">
+        <v>1</v>
+      </c>
+      <c r="J4">
+        <v>1</v>
+      </c>
+      <c r="L4">
+        <v>1</v>
+      </c>
+      <c r="M4">
+        <v>1</v>
+      </c>
+      <c r="N4">
+        <v>1</v>
+      </c>
+      <c r="O4">
+        <v>1</v>
+      </c>
+      <c r="P4">
+        <v>1</v>
+      </c>
+      <c r="Q4">
+        <v>1</v>
+      </c>
+      <c r="S4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>90</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+      <c r="E5">
+        <v>2</v>
+      </c>
+      <c r="F5">
+        <v>3</v>
+      </c>
+      <c r="G5">
+        <v>4</v>
+      </c>
+      <c r="H5">
+        <v>5</v>
+      </c>
+      <c r="J5">
+        <v>6</v>
+      </c>
+      <c r="L5">
+        <v>7</v>
+      </c>
+      <c r="M5">
+        <v>8</v>
+      </c>
+      <c r="N5">
+        <v>9</v>
+      </c>
+      <c r="O5">
+        <v>10</v>
+      </c>
+      <c r="P5">
+        <v>11</v>
+      </c>
+      <c r="Q5">
+        <v>12</v>
+      </c>
+      <c r="S5">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>91</v>
+      </c>
+      <c r="C6">
+        <v>12</v>
+      </c>
+      <c r="D6">
+        <v>11</v>
+      </c>
+      <c r="E6">
+        <v>10</v>
+      </c>
+      <c r="F6">
+        <v>9</v>
+      </c>
+      <c r="G6">
+        <v>8</v>
+      </c>
+      <c r="H6">
+        <v>7</v>
+      </c>
+      <c r="J6">
+        <v>25</v>
+      </c>
+      <c r="L6">
+        <v>6</v>
+      </c>
+      <c r="M6">
+        <v>5</v>
+      </c>
+      <c r="N6">
+        <v>4</v>
+      </c>
+      <c r="O6">
+        <v>3</v>
+      </c>
+      <c r="P6">
+        <v>2</v>
+      </c>
+      <c r="Q6">
+        <v>1</v>
+      </c>
+      <c r="S6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>92</v>
+      </c>
+      <c r="C7">
+        <v>13</v>
+      </c>
+      <c r="D7">
+        <v>14</v>
+      </c>
+      <c r="E7">
+        <v>15</v>
+      </c>
+      <c r="F7">
+        <v>16</v>
+      </c>
+      <c r="G7">
+        <v>17</v>
+      </c>
+      <c r="H7">
+        <v>18</v>
+      </c>
+      <c r="J7" t="s">
+        <v>95</v>
+      </c>
+      <c r="L7">
+        <v>19</v>
+      </c>
+      <c r="M7">
+        <v>20</v>
+      </c>
+      <c r="N7">
+        <v>21</v>
+      </c>
+      <c r="O7">
+        <v>22</v>
+      </c>
+      <c r="P7">
+        <v>23</v>
+      </c>
+      <c r="Q7">
+        <v>25</v>
+      </c>
+      <c r="S7" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>124</v>
+      </c>
+      <c r="E8">
+        <v>5</v>
+      </c>
+      <c r="M8">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>124</v>
+      </c>
+      <c r="C11">
+        <v>1</v>
+      </c>
+      <c r="E11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>88</v>
+      </c>
+      <c r="C12">
+        <v>12</v>
+      </c>
+      <c r="D12">
+        <v>11</v>
+      </c>
+      <c r="E12">
+        <v>10</v>
+      </c>
+      <c r="F12">
+        <v>9</v>
+      </c>
+      <c r="G12">
+        <v>8</v>
+      </c>
+      <c r="H12">
+        <v>7</v>
+      </c>
+      <c r="J12">
+        <v>25</v>
+      </c>
+      <c r="L12">
+        <v>6</v>
+      </c>
+      <c r="M12">
+        <v>5</v>
+      </c>
+      <c r="N12">
+        <v>4</v>
+      </c>
+      <c r="O12">
+        <v>3</v>
+      </c>
+      <c r="P12">
+        <v>2</v>
+      </c>
+      <c r="Q12">
+        <v>1</v>
+      </c>
+      <c r="S12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>89</v>
+      </c>
+      <c r="C13">
+        <v>13</v>
+      </c>
+      <c r="D13">
+        <v>13</v>
+      </c>
+      <c r="E13">
+        <v>13</v>
+      </c>
+      <c r="F13">
+        <v>13</v>
+      </c>
+      <c r="G13">
+        <v>13</v>
+      </c>
+      <c r="H13">
+        <v>13</v>
+      </c>
+      <c r="J13">
+        <v>13</v>
+      </c>
+      <c r="L13">
+        <v>13</v>
+      </c>
+      <c r="M13">
+        <v>13</v>
+      </c>
+      <c r="N13">
+        <v>13</v>
+      </c>
+      <c r="O13">
+        <v>13</v>
+      </c>
+      <c r="P13">
+        <v>13</v>
+      </c>
+      <c r="Q13">
+        <v>13</v>
+      </c>
+      <c r="S13">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>90</v>
+      </c>
+      <c r="C14">
+        <v>0</v>
+      </c>
+      <c r="D14">
+        <v>1</v>
+      </c>
+      <c r="E14">
+        <v>2</v>
+      </c>
+      <c r="F14">
+        <v>3</v>
+      </c>
+      <c r="G14">
+        <v>4</v>
+      </c>
+      <c r="H14">
+        <v>5</v>
+      </c>
+      <c r="J14">
+        <v>6</v>
+      </c>
+      <c r="L14">
+        <v>7</v>
+      </c>
+      <c r="M14">
+        <v>8</v>
+      </c>
+      <c r="N14">
+        <v>9</v>
+      </c>
+      <c r="O14">
+        <v>10</v>
+      </c>
+      <c r="P14">
+        <v>11</v>
+      </c>
+      <c r="Q14">
+        <v>12</v>
+      </c>
+      <c r="S14">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>91</v>
+      </c>
+      <c r="C15">
+        <v>13</v>
+      </c>
+      <c r="D15">
+        <v>14</v>
+      </c>
+      <c r="E15">
+        <v>15</v>
+      </c>
+      <c r="F15">
+        <v>16</v>
+      </c>
+      <c r="G15">
+        <v>17</v>
+      </c>
+      <c r="H15">
+        <v>18</v>
+      </c>
+      <c r="J15" t="s">
+        <v>95</v>
+      </c>
+      <c r="L15">
+        <v>19</v>
+      </c>
+      <c r="M15">
+        <v>20</v>
+      </c>
+      <c r="N15">
+        <v>21</v>
+      </c>
+      <c r="O15">
+        <v>22</v>
+      </c>
+      <c r="P15">
+        <v>23</v>
+      </c>
+      <c r="Q15">
+        <v>24</v>
+      </c>
+      <c r="S15" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>92</v>
+      </c>
+      <c r="C16">
+        <v>12</v>
+      </c>
+      <c r="D16">
+        <v>11</v>
+      </c>
+      <c r="E16">
+        <v>10</v>
+      </c>
+      <c r="F16">
+        <v>9</v>
+      </c>
+      <c r="G16">
+        <v>8</v>
+      </c>
+      <c r="H16">
+        <v>7</v>
+      </c>
+      <c r="J16">
+        <v>25</v>
+      </c>
+      <c r="L16">
+        <v>6</v>
+      </c>
+      <c r="M16">
+        <v>5</v>
+      </c>
+      <c r="N16">
+        <v>4</v>
+      </c>
+      <c r="O16">
+        <v>3</v>
+      </c>
+      <c r="P16">
+        <v>2</v>
+      </c>
+      <c r="Q16">
+        <v>1</v>
+      </c>
+      <c r="S16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>93</v>
+      </c>
+      <c r="J18" t="s">
+        <v>96</v>
+      </c>
+      <c r="S18" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="22" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="C22" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="23" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="E23" t="s">
+        <v>127</v>
+      </c>
+      <c r="F23" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="24" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="C24" t="s">
+        <v>130</v>
+      </c>
+      <c r="E24">
+        <v>20</v>
+      </c>
+      <c r="F24">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="25" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="E25">
+        <v>15</v>
+      </c>
+      <c r="F25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="26" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="E26">
+        <v>12</v>
+      </c>
+      <c r="F26">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="27" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="E27">
+        <v>9</v>
+      </c>
+      <c r="F27">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="28" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="C28" t="s">
+        <v>129</v>
+      </c>
+      <c r="E28">
+        <v>15</v>
+      </c>
+      <c r="F28">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="29" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="E29">
+        <v>12</v>
+      </c>
+      <c r="F29">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="30" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="E30">
+        <v>9</v>
+      </c>
+      <c r="F30">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="31" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="C31" t="s">
+        <v>131</v>
+      </c>
+      <c r="E31">
+        <v>18</v>
+      </c>
+      <c r="F31">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="32" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="E32">
+        <v>12</v>
+      </c>
+      <c r="F32">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="33" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="E33">
+        <v>9</v>
+      </c>
+      <c r="F33">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="34" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C34" t="s">
+        <v>132</v>
+      </c>
+      <c r="E34" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="35" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C35" t="s">
+        <v>134</v>
+      </c>
+      <c r="E35">
+        <v>12</v>
+      </c>
+      <c r="F35">
+        <v>17</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8ECFD8FB-462E-4CB7-B780-C16CB5521A94}">
+  <dimension ref="A1:S35"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>94</v>
+      </c>
+      <c r="J1" t="s">
+        <v>98</v>
+      </c>
+      <c r="S1" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>88</v>
+      </c>
+      <c r="C3">
+        <v>13</v>
+      </c>
+      <c r="D3">
+        <v>14</v>
+      </c>
+      <c r="E3">
+        <v>15</v>
+      </c>
+      <c r="F3">
+        <v>16</v>
+      </c>
+      <c r="G3">
+        <v>17</v>
+      </c>
+      <c r="H3">
+        <v>18</v>
+      </c>
+      <c r="J3">
+        <v>0</v>
+      </c>
+      <c r="L3">
+        <v>19</v>
+      </c>
+      <c r="M3">
+        <v>20</v>
+      </c>
+      <c r="N3">
+        <v>21</v>
+      </c>
+      <c r="O3">
+        <v>22</v>
+      </c>
+      <c r="P3">
+        <v>23</v>
+      </c>
+      <c r="Q3">
+        <v>24</v>
+      </c>
+      <c r="S3">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>89</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+      <c r="E4">
+        <v>1</v>
+      </c>
+      <c r="F4">
+        <v>1</v>
+      </c>
+      <c r="G4">
+        <v>1</v>
+      </c>
+      <c r="H4">
+        <v>1</v>
+      </c>
+      <c r="J4">
+        <v>1</v>
+      </c>
+      <c r="L4">
+        <v>1</v>
+      </c>
+      <c r="M4">
+        <v>1</v>
+      </c>
+      <c r="N4">
+        <v>1</v>
+      </c>
+      <c r="O4">
+        <v>1</v>
+      </c>
+      <c r="P4">
+        <v>1</v>
+      </c>
+      <c r="Q4">
+        <v>1</v>
+      </c>
+      <c r="S4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>90</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+      <c r="E5">
+        <v>2</v>
+      </c>
+      <c r="F5">
+        <v>3</v>
+      </c>
+      <c r="G5">
+        <v>4</v>
+      </c>
+      <c r="H5">
+        <v>5</v>
+      </c>
+      <c r="J5">
+        <v>6</v>
+      </c>
+      <c r="L5">
+        <v>7</v>
+      </c>
+      <c r="M5">
+        <v>8</v>
+      </c>
+      <c r="N5">
+        <v>9</v>
+      </c>
+      <c r="O5">
+        <v>10</v>
+      </c>
+      <c r="P5">
+        <v>11</v>
+      </c>
+      <c r="Q5">
+        <v>12</v>
+      </c>
+      <c r="S5">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>91</v>
+      </c>
+      <c r="C6">
+        <v>12</v>
+      </c>
+      <c r="D6">
+        <v>11</v>
+      </c>
+      <c r="E6">
+        <v>10</v>
+      </c>
+      <c r="F6">
+        <v>9</v>
+      </c>
+      <c r="G6">
+        <v>8</v>
+      </c>
+      <c r="H6">
+        <v>7</v>
+      </c>
+      <c r="J6">
+        <v>25</v>
+      </c>
+      <c r="L6">
+        <v>6</v>
+      </c>
+      <c r="M6">
+        <v>5</v>
+      </c>
+      <c r="N6">
+        <v>4</v>
+      </c>
+      <c r="O6">
+        <v>3</v>
+      </c>
+      <c r="P6">
+        <v>2</v>
+      </c>
+      <c r="Q6">
+        <v>1</v>
+      </c>
+      <c r="S6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>92</v>
+      </c>
+      <c r="C7">
+        <v>13</v>
+      </c>
+      <c r="D7">
+        <v>14</v>
+      </c>
+      <c r="E7">
+        <v>15</v>
+      </c>
+      <c r="F7">
+        <v>16</v>
+      </c>
+      <c r="G7">
+        <v>17</v>
+      </c>
+      <c r="H7">
+        <v>18</v>
+      </c>
+      <c r="J7" t="s">
+        <v>95</v>
+      </c>
+      <c r="L7">
+        <v>19</v>
+      </c>
+      <c r="M7">
+        <v>20</v>
+      </c>
+      <c r="N7">
+        <v>21</v>
+      </c>
+      <c r="O7">
+        <v>22</v>
+      </c>
+      <c r="P7">
+        <v>23</v>
+      </c>
+      <c r="Q7">
+        <v>25</v>
+      </c>
+      <c r="S7" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>124</v>
+      </c>
+      <c r="G8">
+        <v>3</v>
+      </c>
+      <c r="L8">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>124</v>
+      </c>
+      <c r="C11">
+        <v>5</v>
+      </c>
+      <c r="Q11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>88</v>
+      </c>
+      <c r="C12">
+        <v>12</v>
+      </c>
+      <c r="D12">
+        <v>11</v>
+      </c>
+      <c r="E12">
+        <v>10</v>
+      </c>
+      <c r="F12">
+        <v>9</v>
+      </c>
+      <c r="G12">
+        <v>8</v>
+      </c>
+      <c r="H12">
+        <v>7</v>
+      </c>
+      <c r="J12">
+        <v>25</v>
+      </c>
+      <c r="L12">
+        <v>6</v>
+      </c>
+      <c r="M12">
+        <v>5</v>
+      </c>
+      <c r="N12">
+        <v>4</v>
+      </c>
+      <c r="O12">
+        <v>3</v>
+      </c>
+      <c r="P12">
+        <v>2</v>
+      </c>
+      <c r="Q12">
+        <v>1</v>
+      </c>
+      <c r="S12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>89</v>
+      </c>
+      <c r="C13">
+        <v>13</v>
+      </c>
+      <c r="D13">
+        <v>13</v>
+      </c>
+      <c r="E13">
+        <v>13</v>
+      </c>
+      <c r="F13">
+        <v>13</v>
+      </c>
+      <c r="G13">
+        <v>13</v>
+      </c>
+      <c r="H13">
+        <v>13</v>
+      </c>
+      <c r="J13">
+        <v>13</v>
+      </c>
+      <c r="L13">
+        <v>13</v>
+      </c>
+      <c r="M13">
+        <v>13</v>
+      </c>
+      <c r="N13">
+        <v>13</v>
+      </c>
+      <c r="O13">
+        <v>13</v>
+      </c>
+      <c r="P13">
+        <v>13</v>
+      </c>
+      <c r="Q13">
+        <v>13</v>
+      </c>
+      <c r="S13">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>90</v>
+      </c>
+      <c r="C14">
+        <v>0</v>
+      </c>
+      <c r="D14">
+        <v>1</v>
+      </c>
+      <c r="E14">
+        <v>2</v>
+      </c>
+      <c r="F14">
+        <v>3</v>
+      </c>
+      <c r="G14">
+        <v>4</v>
+      </c>
+      <c r="H14">
+        <v>5</v>
+      </c>
+      <c r="J14">
+        <v>6</v>
+      </c>
+      <c r="L14">
+        <v>7</v>
+      </c>
+      <c r="M14">
+        <v>8</v>
+      </c>
+      <c r="N14">
+        <v>9</v>
+      </c>
+      <c r="O14">
+        <v>10</v>
+      </c>
+      <c r="P14">
+        <v>11</v>
+      </c>
+      <c r="Q14">
+        <v>12</v>
+      </c>
+      <c r="S14">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>91</v>
+      </c>
+      <c r="C15">
+        <v>13</v>
+      </c>
+      <c r="D15">
+        <v>14</v>
+      </c>
+      <c r="E15">
+        <v>15</v>
+      </c>
+      <c r="F15">
+        <v>16</v>
+      </c>
+      <c r="G15">
+        <v>17</v>
+      </c>
+      <c r="H15">
+        <v>18</v>
+      </c>
+      <c r="J15" t="s">
+        <v>95</v>
+      </c>
+      <c r="L15">
+        <v>19</v>
+      </c>
+      <c r="M15">
+        <v>20</v>
+      </c>
+      <c r="N15">
+        <v>21</v>
+      </c>
+      <c r="O15">
+        <v>22</v>
+      </c>
+      <c r="P15">
+        <v>23</v>
+      </c>
+      <c r="Q15">
+        <v>24</v>
+      </c>
+      <c r="S15" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>92</v>
+      </c>
+      <c r="C16">
+        <v>12</v>
+      </c>
+      <c r="D16">
+        <v>11</v>
+      </c>
+      <c r="E16">
+        <v>10</v>
+      </c>
+      <c r="F16">
+        <v>9</v>
+      </c>
+      <c r="G16">
+        <v>8</v>
+      </c>
+      <c r="H16">
+        <v>7</v>
+      </c>
+      <c r="J16">
+        <v>25</v>
+      </c>
+      <c r="L16">
+        <v>6</v>
+      </c>
+      <c r="M16">
+        <v>5</v>
+      </c>
+      <c r="N16">
+        <v>4</v>
+      </c>
+      <c r="O16">
+        <v>3</v>
+      </c>
+      <c r="P16">
+        <v>2</v>
+      </c>
+      <c r="Q16">
+        <v>1</v>
+      </c>
+      <c r="S16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>93</v>
+      </c>
+      <c r="J18" t="s">
+        <v>96</v>
+      </c>
+      <c r="S18" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="22" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="C22" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="23" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="E23" t="s">
+        <v>127</v>
+      </c>
+      <c r="F23" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="24" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="C24" t="s">
+        <v>130</v>
+      </c>
+      <c r="E24">
+        <v>20</v>
+      </c>
+      <c r="F24">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="25" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="E25">
+        <v>15</v>
+      </c>
+      <c r="F25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="26" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="E26">
+        <v>12</v>
+      </c>
+      <c r="F26">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="27" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="E27">
+        <v>9</v>
+      </c>
+      <c r="F27">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="28" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="C28" t="s">
+        <v>129</v>
+      </c>
+      <c r="E28">
+        <v>15</v>
+      </c>
+      <c r="F28">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="29" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="E29">
+        <v>12</v>
+      </c>
+      <c r="F29">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="30" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="E30">
+        <v>9</v>
+      </c>
+      <c r="F30">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="31" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="C31" t="s">
+        <v>131</v>
+      </c>
+      <c r="E31">
+        <v>18</v>
+      </c>
+      <c r="F31">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="32" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="E32">
+        <v>12</v>
+      </c>
+      <c r="F32">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="33" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="E33">
+        <v>9</v>
+      </c>
+      <c r="F33">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="34" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C34" t="s">
+        <v>132</v>
+      </c>
+      <c r="E34" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="35" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C35" t="s">
+        <v>134</v>
+      </c>
+      <c r="E35">
+        <v>12</v>
+      </c>
+      <c r="F35">
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>